<commit_message>
Aggiornamento dati Docplanner - Ianiri Informatica - GipoNext - RSA
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111DOCPLANNERX/Ianiri_Informatica/GipoNext/V.5/report-checklist.xlsx
+++ b/GATEWAY/A1#111DOCPLANNERX/Ianiri_Informatica/GipoNext/V.5/report-checklist.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenzo.camerino/Documents/Obsidian notes/GIPO/SSN/Accreditamento GTW/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenzo.camerino/Documents/Obsidian notes/GIPO/SSN/Accreditamento GTW/Accreditamento GipoNext_v1/GATEWAY/A1#111DOCPLANNERX/Ianiri_Informatica/GipoNext/V.5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8676E31C-E5AD-F748-AEB0-A5DBCEE5406C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F640AA93-99C9-1D41-B4FF-996B0DDE3342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19400" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8480" yWindow="500" windowWidth="23820" windowHeight="19400" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -860,12 +860,6 @@
     <t>subject_application_version: v.5</t>
   </si>
   <si>
-    <t>2023-11-27T10:46:59Z</t>
-  </si>
-  <si>
-    <t>7caf6b3ae69223e4</t>
-  </si>
-  <si>
     <t>UNKNOWN_WORKFLOW_ID</t>
   </si>
   <si>
@@ -876,35 +870,11 @@
     <t>Errore gestito dall'operatore di backoffice. Il documento sarà collocato nuovamente nella coda di invio a FSE</t>
   </si>
   <si>
-    <t>2023-11-27T11:29:05Z</t>
-  </si>
-  <si>
-    <t>efde779fff9031fc</t>
-  </si>
-  <si>
     <t>Token JWT non valido.
     Il campo action_id non è valido</t>
   </si>
   <si>
     <t>connection timeout</t>
-  </si>
-  <si>
-    <t>2023-12-07T17:11:35Z</t>
-  </si>
-  <si>
-    <t>1d9743a5dda101c9</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.123456.4.4.5.e30fa6867d5484f24c27a7f98a74a54c6def186e520974c6d3628e1217373a74.0fc741b4e1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-12-07T17:26:55Z</t>
-  </si>
-  <si>
-    <t>b459c624190796c7</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.123456.4.4.5.464946c90f198bf72b19d80d776e61a513280b1e2e9058f535f4da97de0685de.fcab1571f0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">    Errore referto CDA,
@@ -915,15 +885,6 @@
     <t>Errore gestito dall'operatore di backoffice che provvederà a registrare il comune di residenza in anagrafica paziente. Il documento sarà collocato nuovamente nella coda di invio a FSE</t>
   </si>
   <si>
-    <t>2023-12-07T17:45:29Z</t>
-  </si>
-  <si>
-    <t>1642ac2bde4c412b</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.123456.4.4.5.4dee99e626707a48aa9952a8831e60f3331c0a083345a956fdbbc90109b5e122.50699b08a5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Errore referto CDA
     Almeno uno dei seguenti vocaboli non è censito: [CodeSystem: 2.16.840.1.113883.5.1 v2.1.0, Codes: NB</t>
   </si>
@@ -931,15 +892,6 @@
     <t>Errore gestito dall'operatore di backoffice che provvederà a registrare il sesso in anagrafica paziente. Il documento sarà collocato nuovamente nella coda di invio a FSE</t>
   </si>
   <si>
-    <t>2023-12-07T18:15:02Z</t>
-  </si>
-  <si>
-    <t>38a7aa4eec5f7a8c</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.123456.4.4.5.588f0bdc21903563e493249c4a4e31d7908d6b0107b53d3e6b5bebd9268558b9.789d089ee2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>Errore referto CDA
     Sezione Referto: la sezione DEVE essere presente], Sezione Referto: la sezione DEVE contenere un elemento 'text'</t>
   </si>
@@ -947,15 +899,6 @@
     <t>Errore gestito dall'operatore di backoffice che provvederà a valorizzare correttamente la sezione referto. Il documento sarà collocato nuovamente nella coda di invio a FSE</t>
   </si>
   <si>
-    <t>2023-12-07T18:53:18Z</t>
-  </si>
-  <si>
-    <t>01edcbbe86036ad4</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.123456.4.4.5.6271470223afa2a18a34d1baa8b749430664ad026116cadf9abeaef75ef13536.3d81792cf9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>Errore referto CDA 
 Sezione Quesito Diagnostico: la sezione DEVE contenere un elemento 'text'</t>
   </si>
@@ -963,13 +906,70 @@
     <t>Errore gestito dall'operatore di backoffice che provvederà a valorizzare correttamente il quesito diagnostico. Il documento sarà collocato nuovamente nella coda di invio a FSE</t>
   </si>
   <si>
-    <t>2023-12-07T14:57:52Z</t>
-  </si>
-  <si>
-    <t>0b49e14c7c258889</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.123456.4.4.5.9dcddac2f732e0ae5d3de2d44e1b95860fe5839295db5e8c72c8d59f5f224774.b32bd55828^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-12-13T14:34:45Z</t>
+  </si>
+  <si>
+    <t>f1d9f2b5a7426c52</t>
+  </si>
+  <si>
+    <t>2023-12-13T16:49:25Z</t>
+  </si>
+  <si>
+    <t>1d5f14490b92e249</t>
+  </si>
+  <si>
+    <t>2023-12-13T17:17:03Z</t>
+  </si>
+  <si>
+    <t>01baa8983edcec06</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.123456.4.4.5.14dd50d4e940357d0fe86cdf46ee0d39597218f236abcc231d7f8bd726403e06.14d5cd910d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-12-13T17:38:11Z</t>
+  </si>
+  <si>
+    <t>9ae943500bae91cd</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.123456.4.4.5.c86a1c34c156eb48cf78c46fc3c9f3f720ccffe39ac1a7b1cd7bca308861329a.ddce0e143a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-12-13T17:53:11Z</t>
+  </si>
+  <si>
+    <t>e3515c77757f590d</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.123456.4.4.5.ba69b0eac3e070ea0f80d32f77b9f0a5ff3bcf34aabdcf53618201ec9b66e552.9c83539334^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-12-13T18:06:34Z</t>
+  </si>
+  <si>
+    <t>612cd4dd6e75a730</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.123456.4.4.5.a52128d16e2cdae016db35b302b9f9a3aba53218a3fe4c7af5d276761b73f37e.b46900e422^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-12-13T18:19:03Z</t>
+  </si>
+  <si>
+    <t>8f5a2b1b0c9f4718</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.123456.4.4.5.41c2fb746800970dbed7b33870fac5fbfaf80af4f3685353dfd9a70fe8358da1.b557f17801^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-12-13T17:05:43Z</t>
+  </si>
+  <si>
+    <t>b6c5abe355391cb1</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.123456.4.4.5.1419fa86fa686c31cd2aba8452a32f1deb60d7a9f67d8836e588c7dc3aa54bbe.e52aa257d8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -1312,7 +1312,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1405,6 +1405,9 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1427,37 +1430,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3921,10 +3893,10 @@
   <dimension ref="A1:T588"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="129" zoomScaleNormal="129" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="F28" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
+      <selection pane="bottomRight" activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3962,14 +3934,14 @@
       <c r="T1" s="15"/>
     </row>
     <row r="2" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="38" t="s">
+      <c r="B2" s="38"/>
+      <c r="C2" s="39" t="s">
         <v>173</v>
       </c>
-      <c r="D2" s="37"/>
+      <c r="D2" s="38"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -3987,14 +3959,14 @@
       <c r="T2" s="15"/>
     </row>
     <row r="3" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="40"/>
-      <c r="C3" s="45" t="s">
+      <c r="B3" s="41"/>
+      <c r="C3" s="46" t="s">
         <v>174</v>
       </c>
-      <c r="D3" s="37"/>
+      <c r="D3" s="38"/>
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
@@ -4012,12 +3984,12 @@
       <c r="T3" s="15"/>
     </row>
     <row r="4" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="41"/>
-      <c r="B4" s="42"/>
-      <c r="C4" s="45" t="s">
+      <c r="A4" s="42"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="46" t="s">
         <v>175</v>
       </c>
-      <c r="D4" s="37"/>
+      <c r="D4" s="38"/>
       <c r="E4" s="4"/>
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
@@ -4036,12 +4008,12 @@
       <c r="T4" s="15"/>
     </row>
     <row r="5" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="43"/>
-      <c r="B5" s="44"/>
-      <c r="C5" s="45" t="s">
+      <c r="A5" s="44"/>
+      <c r="B5" s="45"/>
+      <c r="C5" s="46" t="s">
         <v>176</v>
       </c>
-      <c r="D5" s="37"/>
+      <c r="D5" s="38"/>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
@@ -4059,8 +4031,8 @@
       <c r="T5" s="15"/>
     </row>
     <row r="6" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="34"/>
-      <c r="B6" s="35"/>
+      <c r="A6" s="35"/>
+      <c r="B6" s="36"/>
       <c r="C6" s="16"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
@@ -4194,16 +4166,16 @@
         <v>56</v>
       </c>
       <c r="F10" s="23">
-        <v>45257</v>
+        <v>45273</v>
       </c>
       <c r="G10" s="24" t="s">
+        <v>190</v>
+      </c>
+      <c r="H10" s="24" t="s">
+        <v>191</v>
+      </c>
+      <c r="I10" s="24" t="s">
         <v>177</v>
-      </c>
-      <c r="H10" s="24" t="s">
-        <v>178</v>
-      </c>
-      <c r="I10" s="24" t="s">
-        <v>179</v>
       </c>
       <c r="J10" s="25" t="s">
         <v>60</v>
@@ -4216,13 +4188,13 @@
         <v>163</v>
       </c>
       <c r="N10" s="25" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="O10" s="25" t="s">
         <v>60</v>
       </c>
       <c r="P10" s="25" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="Q10" s="25"/>
       <c r="R10" s="26"/>
@@ -4248,16 +4220,16 @@
         <v>58</v>
       </c>
       <c r="F11" s="23">
-        <v>45257</v>
+        <v>45273</v>
       </c>
       <c r="G11" s="24" t="s">
-        <v>182</v>
+        <v>192</v>
       </c>
       <c r="H11" s="24" t="s">
-        <v>183</v>
+        <v>193</v>
       </c>
       <c r="I11" s="24" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J11" s="25" t="s">
         <v>60</v>
@@ -4270,13 +4242,13 @@
         <v>163</v>
       </c>
       <c r="N11" s="25" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="O11" s="25" t="s">
         <v>60</v>
       </c>
       <c r="P11" s="25" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="Q11" s="25"/>
       <c r="R11" s="26"/>
@@ -4302,7 +4274,7 @@
         <v>59</v>
       </c>
       <c r="F12" s="23">
-        <v>45257</v>
+        <v>45273</v>
       </c>
       <c r="G12" s="24"/>
       <c r="H12" s="24"/>
@@ -4314,13 +4286,13 @@
       <c r="L12" s="25"/>
       <c r="M12" s="25"/>
       <c r="N12" s="25" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="O12" s="25" t="s">
         <v>60</v>
       </c>
       <c r="P12" s="25" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="Q12" s="25"/>
       <c r="R12" s="26" t="s">
@@ -4348,16 +4320,16 @@
         <v>63</v>
       </c>
       <c r="F13" s="23">
-        <v>45267</v>
+        <v>45273</v>
       </c>
       <c r="G13" s="24" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="H13" s="24" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="I13" s="24" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="J13" s="25" t="s">
         <v>60</v>
@@ -4375,231 +4347,231 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:20" s="56" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="46">
+    <row r="14" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="20">
         <v>148</v>
       </c>
-      <c r="B14" s="47" t="s">
+      <c r="B14" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="C14" s="47" t="s">
+      <c r="C14" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="D14" s="47" t="s">
+      <c r="D14" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="E14" s="48" t="s">
+      <c r="E14" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="F14" s="49"/>
-      <c r="G14" s="50"/>
-      <c r="H14" s="50"/>
-      <c r="I14" s="50"/>
-      <c r="J14" s="51" t="s">
+      <c r="F14" s="23"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="24"/>
+      <c r="J14" s="25" t="s">
         <v>163</v>
       </c>
-      <c r="K14" s="52" t="s">
+      <c r="K14" s="34" t="s">
         <v>164</v>
       </c>
-      <c r="L14" s="51"/>
-      <c r="M14" s="51"/>
-      <c r="N14" s="51"/>
-      <c r="O14" s="51"/>
-      <c r="P14" s="51"/>
-      <c r="Q14" s="51"/>
-      <c r="R14" s="53"/>
-      <c r="S14" s="54"/>
-      <c r="T14" s="55" t="s">
+      <c r="L14" s="25"/>
+      <c r="M14" s="25"/>
+      <c r="N14" s="25"/>
+      <c r="O14" s="25"/>
+      <c r="P14" s="25"/>
+      <c r="Q14" s="25"/>
+      <c r="R14" s="26"/>
+      <c r="S14" s="27"/>
+      <c r="T14" s="28" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:20" s="56" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="46">
+    <row r="15" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="20">
         <v>149</v>
       </c>
-      <c r="B15" s="47" t="s">
+      <c r="B15" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="C15" s="47" t="s">
+      <c r="C15" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="D15" s="47" t="s">
+      <c r="D15" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="E15" s="48" t="s">
+      <c r="E15" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="F15" s="49"/>
-      <c r="G15" s="50"/>
-      <c r="H15" s="50"/>
-      <c r="I15" s="50"/>
-      <c r="J15" s="51" t="s">
+      <c r="F15" s="23"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="24"/>
+      <c r="J15" s="25" t="s">
         <v>163</v>
       </c>
-      <c r="K15" s="52" t="s">
+      <c r="K15" s="34" t="s">
         <v>164</v>
       </c>
-      <c r="L15" s="51"/>
-      <c r="M15" s="51"/>
-      <c r="N15" s="51"/>
-      <c r="O15" s="51"/>
-      <c r="P15" s="51"/>
-      <c r="Q15" s="51"/>
-      <c r="R15" s="53"/>
-      <c r="S15" s="54"/>
-      <c r="T15" s="55" t="s">
+      <c r="L15" s="25"/>
+      <c r="M15" s="25"/>
+      <c r="N15" s="25"/>
+      <c r="O15" s="25"/>
+      <c r="P15" s="25"/>
+      <c r="Q15" s="25"/>
+      <c r="R15" s="26"/>
+      <c r="S15" s="27"/>
+      <c r="T15" s="28" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:20" s="56" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="46">
+    <row r="16" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="20">
         <v>150</v>
       </c>
-      <c r="B16" s="47" t="s">
+      <c r="B16" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="47" t="s">
+      <c r="C16" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="D16" s="47" t="s">
+      <c r="D16" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="E16" s="48" t="s">
+      <c r="E16" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="F16" s="49"/>
-      <c r="G16" s="50"/>
-      <c r="H16" s="50"/>
-      <c r="I16" s="50"/>
-      <c r="J16" s="51" t="s">
+      <c r="F16" s="23"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="24"/>
+      <c r="J16" s="25" t="s">
         <v>163</v>
       </c>
-      <c r="K16" s="52" t="s">
+      <c r="K16" s="34" t="s">
         <v>164</v>
       </c>
-      <c r="L16" s="51"/>
-      <c r="M16" s="51"/>
-      <c r="N16" s="51"/>
-      <c r="O16" s="51"/>
-      <c r="P16" s="51"/>
-      <c r="Q16" s="51"/>
-      <c r="R16" s="53"/>
-      <c r="S16" s="54"/>
-      <c r="T16" s="55" t="s">
+      <c r="L16" s="25"/>
+      <c r="M16" s="25"/>
+      <c r="N16" s="25"/>
+      <c r="O16" s="25"/>
+      <c r="P16" s="25"/>
+      <c r="Q16" s="25"/>
+      <c r="R16" s="26"/>
+      <c r="S16" s="27"/>
+      <c r="T16" s="28" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:20" s="56" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="46">
+    <row r="17" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="20">
         <v>151</v>
       </c>
-      <c r="B17" s="47" t="s">
+      <c r="B17" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="47" t="s">
+      <c r="C17" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="D17" s="47" t="s">
+      <c r="D17" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="E17" s="48" t="s">
+      <c r="E17" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="F17" s="49"/>
-      <c r="G17" s="50"/>
-      <c r="H17" s="50"/>
-      <c r="I17" s="50"/>
-      <c r="J17" s="51" t="s">
+      <c r="F17" s="23"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="25" t="s">
         <v>163</v>
       </c>
-      <c r="K17" s="51" t="s">
+      <c r="K17" s="25" t="s">
         <v>172</v>
       </c>
-      <c r="L17" s="51"/>
-      <c r="M17" s="51"/>
-      <c r="N17" s="51"/>
-      <c r="O17" s="51"/>
-      <c r="P17" s="51"/>
-      <c r="Q17" s="51"/>
-      <c r="R17" s="53"/>
-      <c r="S17" s="54"/>
-      <c r="T17" s="55" t="s">
+      <c r="L17" s="25"/>
+      <c r="M17" s="25"/>
+      <c r="N17" s="25"/>
+      <c r="O17" s="25"/>
+      <c r="P17" s="25"/>
+      <c r="Q17" s="25"/>
+      <c r="R17" s="26"/>
+      <c r="S17" s="27"/>
+      <c r="T17" s="28" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:20" s="56" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="46">
+    <row r="18" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="20">
         <v>152</v>
       </c>
-      <c r="B18" s="47" t="s">
+      <c r="B18" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="C18" s="47" t="s">
+      <c r="C18" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="D18" s="47" t="s">
+      <c r="D18" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="E18" s="48" t="s">
+      <c r="E18" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="F18" s="49"/>
-      <c r="G18" s="50"/>
-      <c r="H18" s="50"/>
-      <c r="I18" s="50"/>
-      <c r="J18" s="51" t="s">
+      <c r="F18" s="23"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="25" t="s">
         <v>163</v>
       </c>
-      <c r="K18" s="52" t="s">
+      <c r="K18" s="34" t="s">
         <v>165</v>
       </c>
-      <c r="L18" s="51"/>
-      <c r="M18" s="51"/>
-      <c r="N18" s="51"/>
-      <c r="O18" s="51"/>
-      <c r="P18" s="51"/>
-      <c r="Q18" s="51"/>
-      <c r="R18" s="53"/>
-      <c r="S18" s="54"/>
-      <c r="T18" s="55" t="s">
+      <c r="L18" s="25"/>
+      <c r="M18" s="25"/>
+      <c r="N18" s="25"/>
+      <c r="O18" s="25"/>
+      <c r="P18" s="25"/>
+      <c r="Q18" s="25"/>
+      <c r="R18" s="26"/>
+      <c r="S18" s="27"/>
+      <c r="T18" s="28" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:20" s="56" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="46">
+    <row r="19" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="20">
         <v>153</v>
       </c>
-      <c r="B19" s="47" t="s">
+      <c r="B19" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="47" t="s">
+      <c r="C19" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="D19" s="47" t="s">
+      <c r="D19" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="E19" s="48" t="s">
+      <c r="E19" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="F19" s="49"/>
-      <c r="G19" s="50"/>
-      <c r="H19" s="50"/>
-      <c r="I19" s="50"/>
-      <c r="J19" s="51" t="s">
+      <c r="F19" s="23"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="25" t="s">
         <v>163</v>
       </c>
-      <c r="K19" s="52" t="s">
+      <c r="K19" s="34" t="s">
         <v>166</v>
       </c>
-      <c r="L19" s="51"/>
-      <c r="M19" s="51"/>
-      <c r="N19" s="51"/>
-      <c r="O19" s="51"/>
-      <c r="P19" s="51"/>
-      <c r="Q19" s="51"/>
-      <c r="R19" s="53"/>
-      <c r="S19" s="54"/>
-      <c r="T19" s="55" t="s">
+      <c r="L19" s="25"/>
+      <c r="M19" s="25"/>
+      <c r="N19" s="25"/>
+      <c r="O19" s="25"/>
+      <c r="P19" s="25"/>
+      <c r="Q19" s="25"/>
+      <c r="R19" s="26"/>
+      <c r="S19" s="27"/>
+      <c r="T19" s="28" t="s">
         <v>52</v>
       </c>
     </row>
@@ -4620,16 +4592,16 @@
         <v>77</v>
       </c>
       <c r="F20" s="23">
-        <v>45267</v>
+        <v>45273</v>
       </c>
       <c r="G20" s="24" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="H20" s="24" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="I20" s="24" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="J20" s="25" t="s">
         <v>60</v>
@@ -4642,13 +4614,13 @@
         <v>60</v>
       </c>
       <c r="N20" s="25" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="O20" s="25" t="s">
         <v>60</v>
       </c>
       <c r="P20" s="25" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="Q20" s="25"/>
       <c r="R20" s="26"/>
@@ -4657,41 +4629,41 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:20" s="56" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="46">
+    <row r="21" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="20">
         <v>155</v>
       </c>
-      <c r="B21" s="47" t="s">
+      <c r="B21" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="C21" s="47" t="s">
+      <c r="C21" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="D21" s="47" t="s">
+      <c r="D21" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="E21" s="48" t="s">
+      <c r="E21" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="F21" s="49"/>
-      <c r="G21" s="50"/>
-      <c r="H21" s="50"/>
-      <c r="I21" s="50"/>
-      <c r="J21" s="51" t="s">
+      <c r="F21" s="23"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="24"/>
+      <c r="J21" s="25" t="s">
         <v>163</v>
       </c>
-      <c r="K21" s="52" t="s">
+      <c r="K21" s="34" t="s">
         <v>166</v>
       </c>
-      <c r="L21" s="51"/>
-      <c r="M21" s="51"/>
-      <c r="N21" s="51"/>
-      <c r="O21" s="51"/>
-      <c r="P21" s="51"/>
-      <c r="Q21" s="51"/>
-      <c r="R21" s="53"/>
-      <c r="S21" s="54"/>
-      <c r="T21" s="55" t="s">
+      <c r="L21" s="25"/>
+      <c r="M21" s="25"/>
+      <c r="N21" s="25"/>
+      <c r="O21" s="25"/>
+      <c r="P21" s="25"/>
+      <c r="Q21" s="25"/>
+      <c r="R21" s="26"/>
+      <c r="S21" s="27"/>
+      <c r="T21" s="28" t="s">
         <v>52</v>
       </c>
     </row>
@@ -4712,16 +4684,16 @@
         <v>81</v>
       </c>
       <c r="F22" s="23">
-        <v>45267</v>
+        <v>45273</v>
       </c>
       <c r="G22" s="24" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="H22" s="24" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="I22" s="24" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="J22" s="25" t="s">
         <v>60</v>
@@ -4734,13 +4706,13 @@
         <v>60</v>
       </c>
       <c r="N22" s="25" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="O22" s="25" t="s">
         <v>60</v>
       </c>
       <c r="P22" s="25" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="Q22" s="25"/>
       <c r="R22" s="26"/>
@@ -4749,155 +4721,155 @@
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="1:20" s="56" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="46">
+    <row r="23" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="20">
         <v>157</v>
       </c>
-      <c r="B23" s="47" t="s">
+      <c r="B23" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="47" t="s">
+      <c r="C23" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="D23" s="47" t="s">
+      <c r="D23" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="E23" s="48" t="s">
+      <c r="E23" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="F23" s="49"/>
-      <c r="G23" s="50"/>
-      <c r="H23" s="50"/>
-      <c r="I23" s="50"/>
-      <c r="J23" s="51" t="s">
+      <c r="F23" s="23"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="24"/>
+      <c r="J23" s="25" t="s">
         <v>163</v>
       </c>
-      <c r="K23" s="52" t="s">
+      <c r="K23" s="34" t="s">
         <v>167</v>
       </c>
-      <c r="L23" s="51"/>
-      <c r="M23" s="51"/>
-      <c r="N23" s="51"/>
-      <c r="O23" s="51"/>
-      <c r="P23" s="51"/>
-      <c r="Q23" s="51"/>
-      <c r="R23" s="53"/>
-      <c r="S23" s="54"/>
-      <c r="T23" s="55" t="s">
+      <c r="L23" s="25"/>
+      <c r="M23" s="25"/>
+      <c r="N23" s="25"/>
+      <c r="O23" s="25"/>
+      <c r="P23" s="25"/>
+      <c r="Q23" s="25"/>
+      <c r="R23" s="26"/>
+      <c r="S23" s="27"/>
+      <c r="T23" s="28" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:20" s="56" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="46">
+    <row r="24" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="20">
         <v>158</v>
       </c>
-      <c r="B24" s="47" t="s">
+      <c r="B24" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="C24" s="47" t="s">
+      <c r="C24" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="D24" s="47" t="s">
+      <c r="D24" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="E24" s="48" t="s">
+      <c r="E24" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="F24" s="49"/>
-      <c r="G24" s="50"/>
-      <c r="H24" s="50"/>
-      <c r="I24" s="50"/>
-      <c r="J24" s="51" t="s">
+      <c r="F24" s="23"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="24"/>
+      <c r="J24" s="25" t="s">
         <v>163</v>
       </c>
-      <c r="K24" s="52" t="s">
+      <c r="K24" s="34" t="s">
         <v>168</v>
       </c>
-      <c r="L24" s="51"/>
-      <c r="M24" s="51"/>
-      <c r="N24" s="51"/>
-      <c r="O24" s="51"/>
-      <c r="P24" s="51"/>
-      <c r="Q24" s="51"/>
-      <c r="R24" s="53"/>
-      <c r="S24" s="54"/>
-      <c r="T24" s="55" t="s">
+      <c r="L24" s="25"/>
+      <c r="M24" s="25"/>
+      <c r="N24" s="25"/>
+      <c r="O24" s="25"/>
+      <c r="P24" s="25"/>
+      <c r="Q24" s="25"/>
+      <c r="R24" s="26"/>
+      <c r="S24" s="27"/>
+      <c r="T24" s="28" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:20" s="56" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="46">
+    <row r="25" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="20">
         <v>159</v>
       </c>
-      <c r="B25" s="47" t="s">
+      <c r="B25" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="C25" s="47" t="s">
+      <c r="C25" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="D25" s="47" t="s">
+      <c r="D25" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="E25" s="48" t="s">
+      <c r="E25" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="F25" s="49"/>
-      <c r="G25" s="50"/>
-      <c r="H25" s="50"/>
-      <c r="I25" s="50"/>
-      <c r="J25" s="51" t="s">
+      <c r="F25" s="23"/>
+      <c r="G25" s="24"/>
+      <c r="H25" s="24"/>
+      <c r="I25" s="24"/>
+      <c r="J25" s="25" t="s">
         <v>163</v>
       </c>
-      <c r="K25" s="52" t="s">
+      <c r="K25" s="34" t="s">
         <v>169</v>
       </c>
-      <c r="L25" s="51"/>
-      <c r="M25" s="51"/>
-      <c r="N25" s="51"/>
-      <c r="O25" s="51"/>
-      <c r="P25" s="51"/>
-      <c r="Q25" s="51"/>
-      <c r="R25" s="53"/>
-      <c r="S25" s="54"/>
-      <c r="T25" s="55" t="s">
+      <c r="L25" s="25"/>
+      <c r="M25" s="25"/>
+      <c r="N25" s="25"/>
+      <c r="O25" s="25"/>
+      <c r="P25" s="25"/>
+      <c r="Q25" s="25"/>
+      <c r="R25" s="26"/>
+      <c r="S25" s="27"/>
+      <c r="T25" s="28" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:20" s="56" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="46">
+    <row r="26" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="20">
         <v>160</v>
       </c>
-      <c r="B26" s="47" t="s">
+      <c r="B26" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="C26" s="47" t="s">
+      <c r="C26" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="D26" s="47" t="s">
+      <c r="D26" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="E26" s="48" t="s">
+      <c r="E26" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="F26" s="49"/>
-      <c r="G26" s="50"/>
-      <c r="H26" s="50"/>
-      <c r="I26" s="50"/>
-      <c r="J26" s="51" t="s">
+      <c r="F26" s="23"/>
+      <c r="G26" s="24"/>
+      <c r="H26" s="24"/>
+      <c r="I26" s="24"/>
+      <c r="J26" s="25" t="s">
         <v>163</v>
       </c>
-      <c r="K26" s="52" t="s">
+      <c r="K26" s="34" t="s">
         <v>170</v>
       </c>
-      <c r="L26" s="51"/>
-      <c r="M26" s="51"/>
-      <c r="N26" s="51"/>
-      <c r="O26" s="51"/>
-      <c r="P26" s="51"/>
-      <c r="Q26" s="51"/>
-      <c r="R26" s="53"/>
-      <c r="S26" s="54"/>
-      <c r="T26" s="55" t="s">
+      <c r="L26" s="25"/>
+      <c r="M26" s="25"/>
+      <c r="N26" s="25"/>
+      <c r="O26" s="25"/>
+      <c r="P26" s="25"/>
+      <c r="Q26" s="25"/>
+      <c r="R26" s="26"/>
+      <c r="S26" s="27"/>
+      <c r="T26" s="28" t="s">
         <v>52</v>
       </c>
     </row>
@@ -4918,16 +4890,16 @@
         <v>91</v>
       </c>
       <c r="F27" s="23">
-        <v>45267</v>
+        <v>45273</v>
       </c>
       <c r="G27" s="24" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="H27" s="24" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="I27" s="24" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="J27" s="25" t="s">
         <v>60</v>
@@ -4940,13 +4912,13 @@
         <v>60</v>
       </c>
       <c r="N27" s="25" t="s">
-        <v>202</v>
+        <v>186</v>
       </c>
       <c r="O27" s="25" t="s">
         <v>60</v>
       </c>
       <c r="P27" s="25" t="s">
-        <v>203</v>
+        <v>187</v>
       </c>
       <c r="Q27" s="25"/>
       <c r="R27" s="26"/>
@@ -4972,16 +4944,16 @@
         <v>93</v>
       </c>
       <c r="F28" s="23">
-        <v>45267</v>
+        <v>45273</v>
       </c>
       <c r="G28" s="24" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="H28" s="24" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="I28" s="24" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="J28" s="25" t="s">
         <v>60</v>
@@ -4994,13 +4966,13 @@
         <v>60</v>
       </c>
       <c r="N28" s="25" t="s">
-        <v>207</v>
+        <v>188</v>
       </c>
       <c r="O28" s="25" t="s">
         <v>60</v>
       </c>
       <c r="P28" s="25" t="s">
-        <v>208</v>
+        <v>189</v>
       </c>
       <c r="Q28" s="25"/>
       <c r="R28" s="26"/>
@@ -5009,269 +4981,269 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:20" s="56" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="46">
+    <row r="29" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="20">
         <v>163</v>
       </c>
-      <c r="B29" s="47" t="s">
+      <c r="B29" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="C29" s="47" t="s">
+      <c r="C29" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="D29" s="47" t="s">
+      <c r="D29" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="E29" s="48" t="s">
+      <c r="E29" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="F29" s="49"/>
-      <c r="G29" s="50"/>
-      <c r="H29" s="50"/>
-      <c r="I29" s="50"/>
-      <c r="J29" s="51" t="s">
+      <c r="F29" s="23"/>
+      <c r="G29" s="24"/>
+      <c r="H29" s="24"/>
+      <c r="I29" s="24"/>
+      <c r="J29" s="25" t="s">
         <v>163</v>
       </c>
-      <c r="K29" s="52" t="s">
+      <c r="K29" s="34" t="s">
         <v>164</v>
       </c>
-      <c r="L29" s="51"/>
-      <c r="M29" s="51"/>
-      <c r="N29" s="51"/>
-      <c r="O29" s="51"/>
-      <c r="P29" s="51"/>
-      <c r="Q29" s="51"/>
-      <c r="R29" s="53"/>
-      <c r="S29" s="54"/>
-      <c r="T29" s="55" t="s">
+      <c r="L29" s="25"/>
+      <c r="M29" s="25"/>
+      <c r="N29" s="25"/>
+      <c r="O29" s="25"/>
+      <c r="P29" s="25"/>
+      <c r="Q29" s="25"/>
+      <c r="R29" s="26"/>
+      <c r="S29" s="27"/>
+      <c r="T29" s="28" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="1:20" s="56" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="46">
+    <row r="30" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="20">
         <v>164</v>
       </c>
-      <c r="B30" s="47" t="s">
+      <c r="B30" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="C30" s="47" t="s">
+      <c r="C30" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="D30" s="47" t="s">
+      <c r="D30" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="E30" s="48" t="s">
+      <c r="E30" s="22" t="s">
         <v>97</v>
       </c>
-      <c r="F30" s="49"/>
-      <c r="G30" s="50"/>
-      <c r="H30" s="50"/>
-      <c r="I30" s="50"/>
-      <c r="J30" s="51" t="s">
+      <c r="F30" s="23"/>
+      <c r="G30" s="24"/>
+      <c r="H30" s="24"/>
+      <c r="I30" s="24"/>
+      <c r="J30" s="25" t="s">
         <v>163</v>
       </c>
-      <c r="K30" s="52" t="s">
+      <c r="K30" s="34" t="s">
         <v>164</v>
       </c>
-      <c r="L30" s="51"/>
-      <c r="M30" s="51"/>
-      <c r="N30" s="51"/>
-      <c r="O30" s="51"/>
-      <c r="P30" s="51"/>
-      <c r="Q30" s="51"/>
-      <c r="R30" s="53"/>
-      <c r="S30" s="54"/>
-      <c r="T30" s="55" t="s">
+      <c r="L30" s="25"/>
+      <c r="M30" s="25"/>
+      <c r="N30" s="25"/>
+      <c r="O30" s="25"/>
+      <c r="P30" s="25"/>
+      <c r="Q30" s="25"/>
+      <c r="R30" s="26"/>
+      <c r="S30" s="27"/>
+      <c r="T30" s="28" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="31" spans="1:20" s="56" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="46">
+    <row r="31" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="20">
         <v>165</v>
       </c>
-      <c r="B31" s="47" t="s">
+      <c r="B31" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="C31" s="47" t="s">
+      <c r="C31" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="D31" s="47" t="s">
+      <c r="D31" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="E31" s="48" t="s">
+      <c r="E31" s="22" t="s">
         <v>99</v>
       </c>
-      <c r="F31" s="49"/>
-      <c r="G31" s="50"/>
-      <c r="H31" s="50"/>
-      <c r="I31" s="50"/>
-      <c r="J31" s="51" t="s">
+      <c r="F31" s="23"/>
+      <c r="G31" s="24"/>
+      <c r="H31" s="24"/>
+      <c r="I31" s="24"/>
+      <c r="J31" s="25" t="s">
         <v>163</v>
       </c>
-      <c r="K31" s="52" t="s">
+      <c r="K31" s="34" t="s">
         <v>164</v>
       </c>
-      <c r="L31" s="51"/>
-      <c r="M31" s="51"/>
-      <c r="N31" s="51"/>
-      <c r="O31" s="51"/>
-      <c r="P31" s="51"/>
-      <c r="Q31" s="51"/>
-      <c r="R31" s="53"/>
-      <c r="S31" s="54"/>
-      <c r="T31" s="55" t="s">
+      <c r="L31" s="25"/>
+      <c r="M31" s="25"/>
+      <c r="N31" s="25"/>
+      <c r="O31" s="25"/>
+      <c r="P31" s="25"/>
+      <c r="Q31" s="25"/>
+      <c r="R31" s="26"/>
+      <c r="S31" s="27"/>
+      <c r="T31" s="28" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="32" spans="1:20" s="56" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="46">
+    <row r="32" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="20">
         <v>166</v>
       </c>
-      <c r="B32" s="47" t="s">
+      <c r="B32" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="C32" s="47" t="s">
+      <c r="C32" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="D32" s="47" t="s">
+      <c r="D32" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="E32" s="48" t="s">
+      <c r="E32" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="F32" s="49"/>
-      <c r="G32" s="50"/>
-      <c r="H32" s="50"/>
-      <c r="I32" s="50"/>
-      <c r="J32" s="51" t="s">
+      <c r="F32" s="23"/>
+      <c r="G32" s="24"/>
+      <c r="H32" s="24"/>
+      <c r="I32" s="24"/>
+      <c r="J32" s="25" t="s">
         <v>163</v>
       </c>
-      <c r="K32" s="52" t="s">
+      <c r="K32" s="34" t="s">
         <v>164</v>
       </c>
-      <c r="L32" s="51"/>
-      <c r="M32" s="51"/>
-      <c r="N32" s="51"/>
-      <c r="O32" s="51"/>
-      <c r="P32" s="51"/>
-      <c r="Q32" s="51"/>
-      <c r="R32" s="53"/>
-      <c r="S32" s="54"/>
-      <c r="T32" s="55" t="s">
+      <c r="L32" s="25"/>
+      <c r="M32" s="25"/>
+      <c r="N32" s="25"/>
+      <c r="O32" s="25"/>
+      <c r="P32" s="25"/>
+      <c r="Q32" s="25"/>
+      <c r="R32" s="26"/>
+      <c r="S32" s="27"/>
+      <c r="T32" s="28" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="33" spans="1:20" s="56" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="46">
+    <row r="33" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="20">
         <v>167</v>
       </c>
-      <c r="B33" s="47" t="s">
+      <c r="B33" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="C33" s="47" t="s">
+      <c r="C33" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="D33" s="47" t="s">
+      <c r="D33" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="E33" s="48" t="s">
+      <c r="E33" s="22" t="s">
         <v>103</v>
       </c>
-      <c r="F33" s="49"/>
-      <c r="G33" s="50"/>
-      <c r="H33" s="50"/>
-      <c r="I33" s="50"/>
-      <c r="J33" s="51" t="s">
+      <c r="F33" s="23"/>
+      <c r="G33" s="24"/>
+      <c r="H33" s="24"/>
+      <c r="I33" s="24"/>
+      <c r="J33" s="25" t="s">
         <v>163</v>
       </c>
-      <c r="K33" s="52" t="s">
+      <c r="K33" s="34" t="s">
         <v>164</v>
       </c>
-      <c r="L33" s="51"/>
-      <c r="M33" s="51"/>
-      <c r="N33" s="51"/>
-      <c r="O33" s="51"/>
-      <c r="P33" s="51"/>
-      <c r="Q33" s="51"/>
-      <c r="R33" s="53"/>
-      <c r="S33" s="54"/>
-      <c r="T33" s="55" t="s">
+      <c r="L33" s="25"/>
+      <c r="M33" s="25"/>
+      <c r="N33" s="25"/>
+      <c r="O33" s="25"/>
+      <c r="P33" s="25"/>
+      <c r="Q33" s="25"/>
+      <c r="R33" s="26"/>
+      <c r="S33" s="27"/>
+      <c r="T33" s="28" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="34" spans="1:20" s="56" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="46">
+    <row r="34" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="20">
         <v>168</v>
       </c>
-      <c r="B34" s="47" t="s">
+      <c r="B34" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="C34" s="47" t="s">
+      <c r="C34" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="D34" s="47" t="s">
+      <c r="D34" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="E34" s="48" t="s">
+      <c r="E34" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="F34" s="49"/>
-      <c r="G34" s="50"/>
-      <c r="H34" s="50"/>
-      <c r="I34" s="50"/>
-      <c r="J34" s="51" t="s">
+      <c r="F34" s="23"/>
+      <c r="G34" s="24"/>
+      <c r="H34" s="24"/>
+      <c r="I34" s="24"/>
+      <c r="J34" s="25" t="s">
         <v>163</v>
       </c>
-      <c r="K34" s="52" t="s">
+      <c r="K34" s="34" t="s">
         <v>164</v>
       </c>
-      <c r="L34" s="51"/>
-      <c r="M34" s="51"/>
-      <c r="N34" s="51"/>
-      <c r="O34" s="51"/>
-      <c r="P34" s="51"/>
-      <c r="Q34" s="51"/>
-      <c r="R34" s="53"/>
-      <c r="S34" s="54"/>
-      <c r="T34" s="55" t="s">
+      <c r="L34" s="25"/>
+      <c r="M34" s="25"/>
+      <c r="N34" s="25"/>
+      <c r="O34" s="25"/>
+      <c r="P34" s="25"/>
+      <c r="Q34" s="25"/>
+      <c r="R34" s="26"/>
+      <c r="S34" s="27"/>
+      <c r="T34" s="28" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="35" spans="1:20" s="56" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="46">
+    <row r="35" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="20">
         <v>169</v>
       </c>
-      <c r="B35" s="47" t="s">
+      <c r="B35" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="C35" s="47" t="s">
+      <c r="C35" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="D35" s="47" t="s">
+      <c r="D35" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="E35" s="48" t="s">
+      <c r="E35" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="F35" s="49"/>
-      <c r="G35" s="50"/>
-      <c r="H35" s="50"/>
-      <c r="I35" s="50"/>
-      <c r="J35" s="51" t="s">
+      <c r="F35" s="23"/>
+      <c r="G35" s="24"/>
+      <c r="H35" s="24"/>
+      <c r="I35" s="24"/>
+      <c r="J35" s="25" t="s">
         <v>163</v>
       </c>
-      <c r="K35" s="52" t="s">
+      <c r="K35" s="34" t="s">
         <v>171</v>
       </c>
-      <c r="L35" s="51"/>
-      <c r="M35" s="51"/>
-      <c r="N35" s="51"/>
-      <c r="O35" s="51"/>
-      <c r="P35" s="51"/>
-      <c r="Q35" s="51"/>
-      <c r="R35" s="53"/>
-      <c r="S35" s="54"/>
-      <c r="T35" s="55" t="s">
+      <c r="L35" s="25"/>
+      <c r="M35" s="25"/>
+      <c r="N35" s="25"/>
+      <c r="O35" s="25"/>
+      <c r="P35" s="25"/>
+      <c r="Q35" s="25"/>
+      <c r="R35" s="26"/>
+      <c r="S35" s="27"/>
+      <c r="T35" s="28" t="s">
         <v>52</v>
       </c>
     </row>
@@ -5292,7 +5264,7 @@
         <v>109</v>
       </c>
       <c r="F36" s="23">
-        <v>45267</v>
+        <v>45273</v>
       </c>
       <c r="G36" s="24" t="s">
         <v>209</v>

</xml_diff>

<commit_message>
Aggiornamento checklist per refuso
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111DOCPLANNERX/Ianiri_Informatica/GipoNext/V.5/report-checklist.xlsx
+++ b/GATEWAY/A1#111DOCPLANNERX/Ianiri_Informatica/GipoNext/V.5/report-checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenzo.camerino/Documents/Obsidian notes/GIPO/SSN/Accreditamento GTW/Accreditamento GipoNext_v1/GATEWAY/A1#111DOCPLANNERX/Ianiri_Informatica/GipoNext/V.5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F640AA93-99C9-1D41-B4FF-996B0DDE3342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{573FBA59-2F9C-5449-952C-43073CAA8967}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8480" yWindow="500" windowWidth="23820" windowHeight="19400" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19400" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="213">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -970,6 +970,9 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.123456.4.4.5.1419fa86fa686c31cd2aba8452a32f1deb60d7a9f67d8836e588c7dc3aa54bbe.e52aa257d8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>L'applicativo non consente la registrazione di pazienti senza nome o cognome</t>
   </si>
 </sst>
 </file>
@@ -3893,10 +3896,10 @@
   <dimension ref="A1:T588"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="129" zoomScaleNormal="129" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="F28" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="F20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="I36" sqref="I36"/>
+      <selection pane="bottomRight" activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3908,7 +3911,8 @@
     <col min="5" max="5" width="104.83203125" customWidth="1"/>
     <col min="6" max="9" width="33.1640625" customWidth="1"/>
     <col min="10" max="10" width="27.1640625" customWidth="1"/>
-    <col min="11" max="15" width="36.5" customWidth="1"/>
+    <col min="11" max="11" width="54.33203125" customWidth="1"/>
+    <col min="12" max="15" width="36.5" customWidth="1"/>
     <col min="16" max="16" width="27.1640625" customWidth="1"/>
     <col min="17" max="17" width="33.1640625" customWidth="1"/>
     <col min="18" max="18" width="36.5" customWidth="1"/>
@@ -4652,8 +4656,8 @@
       <c r="J21" s="25" t="s">
         <v>163</v>
       </c>
-      <c r="K21" s="34" t="s">
-        <v>166</v>
+      <c r="K21" s="25" t="s">
+        <v>212</v>
       </c>
       <c r="L21" s="25"/>
       <c r="M21" s="25"/>

</xml_diff>